<commit_message>
add raceCode + lifeTable technical notes
</commit_message>
<xml_diff>
--- a/myCCB/myInfo/icd10_to_CAUSE.xlsx
+++ b/myCCB/myInfo/icd10_to_CAUSE.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB\myCCB\myInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B41149-69BE-4832-B045-5F44E2757626}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$1:$W$226</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,14 +38,14 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Dauphine, David (CDPH-CHSI-PHPRB)</author>
     <author>Matt</author>
     <author>Dauphine, David (CDPH-CHSI)</author>
   </authors>
   <commentList>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -70,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C57" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="C57" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -94,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R126" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="R126" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -123,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2685" uniqueCount="1455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2686" uniqueCount="1456">
   <si>
     <t>I. Communicable, maternal, perinatal and nutritional conditions</t>
   </si>
@@ -4649,11 +4648,14 @@
   <si>
     <t>Food-borne trematodes</t>
   </si>
+  <si>
+    <t>Homicide</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###0.;###0."/>
   </numFmts>
@@ -5215,7 +5217,7 @@
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5438,23 +5440,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -5490,23 +5475,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5682,14 +5650,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W234"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B159" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B219" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E168" sqref="E168"/>
+      <selection pane="bottomRight" activeCell="E224" sqref="E224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -13308,7 +13276,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="136" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A136" s="42" t="str">
         <f t="shared" si="12"/>
         <v>...D.06. - Alzheimer’s disease and other dementias</v>
@@ -15702,7 +15670,7 @@
       </c>
       <c r="W176" s="2"/>
     </row>
-    <row r="177" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A177" s="42" t="str">
         <f t="shared" si="12"/>
         <v>....D.10.c. - Other chronic kidney disease</v>
@@ -15766,7 +15734,7 @@
       </c>
       <c r="W177" s="2"/>
     </row>
-    <row r="178" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A178" s="42" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -16374,7 +16342,7 @@
       </c>
       <c r="W188" s="2"/>
     </row>
-    <row r="189" spans="1:23" ht="51" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:23" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A189" s="42" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -16722,7 +16690,7 @@
       </c>
       <c r="W194" s="2"/>
     </row>
-    <row r="195" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A195" s="42" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -17343,7 +17311,7 @@
     </row>
     <row r="207" spans="1:23" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A207" s="42" t="str">
-        <f>IF(J207&lt;&gt;"",IF(H207&lt;&gt;"",CONCATENATE("....",F207,".",G207,".",H207,". - ",D207),IF(G207&lt;&gt;"",CONCATENATE("...",F207,".",G207,". - ",D207),CONCATENATE("..",F207,". - ",D207))),"")</f>
+        <f t="shared" ref="A207:A212" si="24">IF(J207&lt;&gt;"",IF(H207&lt;&gt;"",CONCATENATE("....",F207,".",G207,".",H207,". - ",D207),IF(G207&lt;&gt;"",CONCATENATE("...",F207,".",G207,". - ",D207),CONCATENATE("..",F207,". - ",D207))),"")</f>
         <v/>
       </c>
       <c r="B207" s="2">
@@ -17393,7 +17361,7 @@
     </row>
     <row r="208" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A208" s="42" t="str">
-        <f>IF(J208&lt;&gt;"",IF(H208&lt;&gt;"",CONCATENATE("....",F208,".",G208,".",H208,". - ",D208),IF(G208&lt;&gt;"",CONCATENATE("...",F208,".",G208,". - ",D208),CONCATENATE("..",F208,". - ",D208))),"")</f>
+        <f t="shared" si="24"/>
         <v>....E.02.a. - Opioid use disorders</v>
       </c>
       <c r="B208" s="2">
@@ -17455,7 +17423,7 @@
     </row>
     <row r="209" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A209" s="42" t="str">
-        <f>IF(J209&lt;&gt;"",IF(H209&lt;&gt;"",CONCATENATE("....",F209,".",G209,".",H209,". - ",D209),IF(G209&lt;&gt;"",CONCATENATE("...",F209,".",G209,". - ",D209),CONCATENATE("..",F209,". - ",D209))),"")</f>
+        <f t="shared" si="24"/>
         <v>....E.02.b. - Cocaine use disorders</v>
       </c>
       <c r="B209" s="2">
@@ -17517,7 +17485,7 @@
     </row>
     <row r="210" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A210" s="42" t="str">
-        <f>IF(J210&lt;&gt;"",IF(H210&lt;&gt;"",CONCATENATE("....",F210,".",G210,".",H210,". - ",D210),IF(G210&lt;&gt;"",CONCATENATE("...",F210,".",G210,". - ",D210),CONCATENATE("..",F210,". - ",D210))),"")</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="B210" s="2">
@@ -17569,7 +17537,7 @@
     </row>
     <row r="211" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A211" s="42" t="str">
-        <f>IF(J211&lt;&gt;"",IF(H211&lt;&gt;"",CONCATENATE("....",F211,".",G211,".",H211,". - ",D211),IF(G211&lt;&gt;"",CONCATENATE("...",F211,".",G211,". - ",D211),CONCATENATE("..",F211,". - ",D211))),"")</f>
+        <f t="shared" si="24"/>
         <v>....E.02.c. - Other stimulant use disorders</v>
       </c>
       <c r="B211" s="2">
@@ -17631,7 +17599,7 @@
     </row>
     <row r="212" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A212" s="42" t="str">
-        <f>IF(J212&lt;&gt;"",IF(H212&lt;&gt;"",CONCATENATE("....",F212,".",G212,".",H212,". - ",D212),IF(G212&lt;&gt;"",CONCATENATE("...",F212,".",G212,". - ",D212),CONCATENATE("..",F212,". - ",D212))),"")</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="B212" s="2">
@@ -17816,7 +17784,7 @@
       </c>
       <c r="W214" s="2"/>
     </row>
-    <row r="215" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A215" s="42" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -18089,7 +18057,7 @@
       </c>
       <c r="W219" s="2"/>
     </row>
-    <row r="220" spans="1:23" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:23" ht="51" x14ac:dyDescent="0.25">
       <c r="A220" s="42" t="str">
         <f t="shared" si="20"/>
         <v>...E.05. - Other unintentional injuries</v>
@@ -18228,7 +18196,7 @@
       </c>
       <c r="H222" s="6"/>
       <c r="I222" s="38" t="str">
-        <f t="shared" ref="I222:I229" si="24">CONCATENATE("c",F222,G222,H222)</f>
+        <f t="shared" ref="I222:I229" si="25">CONCATENATE("c",F222,G222,H222)</f>
         <v>cE07</v>
       </c>
       <c r="J222" s="38" t="str">
@@ -18283,7 +18251,9 @@
       <c r="D223" s="5" t="s">
         <v>1261</v>
       </c>
-      <c r="E223" s="72"/>
+      <c r="E223" s="72" t="s">
+        <v>1455</v>
+      </c>
       <c r="F223" s="6" t="s">
         <v>1135</v>
       </c>
@@ -18324,7 +18294,7 @@
       </c>
       <c r="W223" s="2"/>
     </row>
-    <row r="224" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A224" s="42" t="str">
         <f t="shared" si="20"/>
         <v>....E.08.a. - Homicide excluding legal intervention</v>
@@ -18345,11 +18315,11 @@
         <v>1123</v>
       </c>
       <c r="I224" s="38" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>cE08a</v>
       </c>
       <c r="J224" s="38" t="str">
-        <f t="shared" ref="J224:J227" si="25">CONCATENATE(F224,G224,H224)</f>
+        <f t="shared" ref="J224:J227" si="26">CONCATENATE(F224,G224,H224)</f>
         <v>E08a</v>
       </c>
       <c r="K224" s="5" t="s">
@@ -18393,11 +18363,11 @@
         <v>1124</v>
       </c>
       <c r="I225" s="38" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>cE08b</v>
       </c>
       <c r="J225" s="38" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>E08b</v>
       </c>
       <c r="K225" s="5" t="s">
@@ -18422,7 +18392,7 @@
       <c r="V225" s="43"/>
       <c r="W225" s="2"/>
     </row>
-    <row r="226" spans="1:23" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:23" ht="102" x14ac:dyDescent="0.25">
       <c r="A226" s="42" t="str">
         <f t="shared" si="20"/>
         <v>....E.08.c. - Execution, War, Terrorism</v>
@@ -18447,11 +18417,11 @@
         <v>1126</v>
       </c>
       <c r="I226" s="38" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>cE08c</v>
       </c>
       <c r="J226" s="38" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>E08c</v>
       </c>
       <c r="K226" s="5" t="s">
@@ -18508,11 +18478,11 @@
         <v>1216</v>
       </c>
       <c r="I227" s="38" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>cE99</v>
       </c>
       <c r="J227" s="38" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>E99</v>
       </c>
       <c r="K227" s="46" t="s">
@@ -18546,7 +18516,7 @@
         <v>1136</v>
       </c>
       <c r="I228" s="38" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>cZ01</v>
       </c>
       <c r="J228" s="38" t="str">
@@ -18566,7 +18536,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="229" spans="1:23" ht="51" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:23" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A229" s="42" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -18581,7 +18551,7 @@
         <v>1144</v>
       </c>
       <c r="I229" s="40" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>cA09</v>
       </c>
       <c r="J229" s="38"/>
@@ -18614,11 +18584,11 @@
       </c>
       <c r="I230" s="41"/>
       <c r="J230" s="38" t="str">
-        <f t="shared" ref="J230:J232" si="26">CONCATENATE(F230,G230,H230)</f>
+        <f t="shared" ref="J230:J232" si="27">CONCATENATE(F230,G230,H230)</f>
         <v>Z02</v>
       </c>
     </row>
-    <row r="231" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:23" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A231" s="42" t="str">
         <f t="shared" si="20"/>
         <v>...Z.03. - Code does not map</v>
@@ -18634,7 +18604,7 @@
       </c>
       <c r="I231" s="41"/>
       <c r="J231" s="38" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>Z03</v>
       </c>
       <c r="K231" s="16" t="s">
@@ -18654,7 +18624,7 @@
       </c>
       <c r="I232" s="41"/>
       <c r="J232" s="38" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>Z</v>
       </c>
     </row>
@@ -18664,7 +18634,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W226" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:W226"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -18677,7 +18647,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18872,7 +18842,7 @@
     <row r="17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -18885,7 +18855,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J19"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">

</xml_diff>

<commit_message>
race color standards; add groupQuarter script and RDS; remove level 3 drug disorders from causeList
</commit_message>
<xml_diff>
--- a/myCCB/myInfo/icd10_to_CAUSE.xlsx
+++ b/myCCB/myInfo/icd10_to_CAUSE.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB\myCCB\myInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E70776-3C71-4603-AC9F-820C4A9D0D41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -22,12 +23,14 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$1:$W$226</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -38,14 +41,14 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Dauphine, David (CDPH-CHSI-PHPRB)</author>
     <author>Matt</author>
     <author>Dauphine, David (CDPH-CHSI)</author>
   </authors>
   <commentList>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -69,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C57" authorId="1" shapeId="0">
+    <comment ref="C57" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -93,7 +96,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R126" authorId="2" shapeId="0">
+    <comment ref="R126" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -122,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2686" uniqueCount="1456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2683" uniqueCount="1456">
   <si>
     <t>I. Communicable, maternal, perinatal and nutritional conditions</t>
   </si>
@@ -4655,7 +4658,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###0.;###0."/>
   </numFmts>
@@ -5217,7 +5220,7 @@
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5440,6 +5443,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -5475,6 +5495,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5650,14 +5687,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W234"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B219" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B205" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E224" sqref="E224"/>
+      <selection pane="bottomRight" activeCell="H208" sqref="H208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -17362,7 +17399,7 @@
     <row r="208" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A208" s="42" t="str">
         <f t="shared" si="24"/>
-        <v>....E.02.a. - Opioid use disorders</v>
+        <v/>
       </c>
       <c r="B208" s="2">
         <v>118</v>
@@ -17380,17 +17417,12 @@
       <c r="G208" s="26" t="s">
         <v>1137</v>
       </c>
-      <c r="H208" s="6" t="s">
-        <v>1123</v>
-      </c>
+      <c r="H208" s="6"/>
       <c r="I208" s="38" t="str">
         <f>CONCATENATE("c",F208,G208,H208)</f>
-        <v>cE02a</v>
-      </c>
-      <c r="J208" s="38" t="str">
-        <f>CONCATENATE(F208,G208,H208)</f>
-        <v>E02a</v>
-      </c>
+        <v>cE02</v>
+      </c>
+      <c r="J208" s="38"/>
       <c r="K208" s="5"/>
       <c r="L208" s="5"/>
       <c r="M208" s="5" t="s">
@@ -17424,7 +17456,7 @@
     <row r="209" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A209" s="42" t="str">
         <f t="shared" si="24"/>
-        <v>....E.02.b. - Cocaine use disorders</v>
+        <v/>
       </c>
       <c r="B209" s="2">
         <v>119</v>
@@ -17442,17 +17474,12 @@
       <c r="G209" s="26" t="s">
         <v>1137</v>
       </c>
-      <c r="H209" s="6" t="s">
-        <v>1124</v>
-      </c>
+      <c r="H209" s="6"/>
       <c r="I209" s="38" t="str">
         <f>CONCATENATE("c",F209,G209,H209)</f>
-        <v>cE02b</v>
-      </c>
-      <c r="J209" s="38" t="str">
-        <f>CONCATENATE(F209,G209,H209)</f>
-        <v>E02b</v>
-      </c>
+        <v>cE02</v>
+      </c>
+      <c r="J209" s="38"/>
       <c r="K209" s="5"/>
       <c r="L209" s="5"/>
       <c r="M209" s="5" t="s">
@@ -17538,7 +17565,7 @@
     <row r="211" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A211" s="42" t="str">
         <f t="shared" si="24"/>
-        <v>....E.02.c. - Other stimulant use disorders</v>
+        <v/>
       </c>
       <c r="B211" s="2">
         <v>120</v>
@@ -17556,17 +17583,12 @@
       <c r="G211" s="26" t="s">
         <v>1137</v>
       </c>
-      <c r="H211" s="6" t="s">
-        <v>1126</v>
-      </c>
+      <c r="H211" s="6"/>
       <c r="I211" s="38" t="str">
         <f>CONCATENATE("c",F211,G211,H211)</f>
-        <v>cE02c</v>
-      </c>
-      <c r="J211" s="38" t="str">
-        <f>CONCATENATE(F211,G211,H211)</f>
-        <v>E02c</v>
-      </c>
+        <v>cE02</v>
+      </c>
+      <c r="J211" s="38"/>
       <c r="K211" s="5"/>
       <c r="L211" s="5"/>
       <c r="M211" s="5" t="s">
@@ -18634,7 +18656,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W226"/>
+  <autoFilter ref="A1:W226" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -18647,7 +18669,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18842,7 +18864,7 @@
     <row r="17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -18855,7 +18877,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:J19"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">

</xml_diff>

<commit_message>
October push - Update xMDA, add SOPH, etc
</commit_message>
<xml_diff>
--- a/myCCB/myInfo/icd10_to_CAUSE.xlsx
+++ b/myCCB/myInfo/icd10_to_CAUSE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB\myCCB\myInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA28F118-C452-463C-A094-7394F1CE26E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8E25D1-C384-4E4B-BA1C-FA9B3F388B73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -5728,42 +5728,40 @@
   <dimension ref="A1:W234"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F87" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B130" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M90" sqref="M90"/>
+      <selection pane="bottomRight" activeCell="A205" sqref="A205"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="49" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.140625" style="42" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" style="44" customWidth="1"/>
-    <col min="3" max="3" width="26" style="42" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="46" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="16" customWidth="1"/>
-    <col min="6" max="6" width="4.42578125" style="52" customWidth="1"/>
-    <col min="7" max="7" width="3.7109375" style="51" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" style="52" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" style="52" customWidth="1"/>
-    <col min="10" max="10" width="8" style="52" customWidth="1"/>
-    <col min="11" max="11" width="29.28515625" style="16" customWidth="1"/>
-    <col min="12" max="12" width="10" style="46" customWidth="1"/>
-    <col min="13" max="13" width="28" style="16" customWidth="1"/>
-    <col min="14" max="14" width="38.140625" style="16" customWidth="1"/>
-    <col min="15" max="15" width="27.5703125" style="16" customWidth="1"/>
-    <col min="16" max="16" width="71.28515625" style="16" customWidth="1"/>
-    <col min="17" max="17" width="16.42578125" style="61" customWidth="1"/>
-    <col min="18" max="18" width="35.140625" style="61" customWidth="1"/>
-    <col min="19" max="19" width="62.140625" style="70" customWidth="1"/>
-    <col min="20" max="20" width="40.7109375" style="70" customWidth="1"/>
-    <col min="21" max="21" width="50.85546875" style="44" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="50.85546875" style="44" customWidth="1"/>
-    <col min="23" max="23" width="50.42578125" style="44" customWidth="1"/>
-    <col min="24" max="16384" width="8.85546875" style="44"/>
+    <col min="1" max="1" width="48.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4" style="44" customWidth="1"/>
+    <col min="3" max="3" width="47.5703125" style="42" customWidth="1"/>
+    <col min="4" max="4" width="47.85546875" style="46" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" style="52" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" style="51" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" style="52" customWidth="1"/>
+    <col min="9" max="10" width="7.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="63.140625" style="16" customWidth="1"/>
+    <col min="12" max="12" width="27.28515625" style="46" customWidth="1"/>
+    <col min="13" max="14" width="49" style="16"/>
+    <col min="15" max="15" width="48.85546875" style="16" customWidth="1"/>
+    <col min="16" max="16" width="46.28515625" style="16" customWidth="1"/>
+    <col min="17" max="17" width="49" style="61" customWidth="1"/>
+    <col min="18" max="18" width="48.85546875" style="61" customWidth="1"/>
+    <col min="19" max="19" width="61.5703125" style="70" customWidth="1"/>
+    <col min="20" max="20" width="49" style="70" customWidth="1"/>
+    <col min="21" max="21" width="51.5703125" style="44" customWidth="1"/>
+    <col min="22" max="22" width="53" style="44" customWidth="1"/>
+    <col min="23" max="23" width="97" style="44" customWidth="1"/>
+    <col min="24" max="16384" width="49" style="44"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="16" t="s">
         <v>1150</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -5834,7 +5832,7 @@
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="str">
+      <c r="A2" s="16" t="str">
         <f>CONCATENATE(".",U2)</f>
         <v>.All CAUSES</v>
       </c>
@@ -5877,7 +5875,7 @@
       <c r="W2" s="6"/>
     </row>
     <row r="3" spans="1:23" ht="41.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="str">
+      <c r="A3" s="16" t="str">
         <f t="shared" ref="A3:A65" si="0">IF(J3&lt;&gt;"",IF(H3&lt;&gt;"",CONCATENATE("....",F3,".",G3,".",H3,". - ",D3),IF(G3&lt;&gt;"",CONCATENATE("...",F3,".",G3,". - ",D3),CONCATENATE("..",F3,". - ",D3))),"")</f>
         <v>..A. - Communicable, maternal, perinatal and nutritional conditions</v>
       </c>
@@ -5928,7 +5926,7 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="str">
+      <c r="A4" s="16" t="str">
         <f t="shared" si="0"/>
         <v>...A.99. - Other Infectious Diseases/Nutritional Deficiencies</v>
       </c>
@@ -5971,7 +5969,7 @@
       <c r="W4" s="2"/>
     </row>
     <row r="5" spans="1:23" ht="24" x14ac:dyDescent="0.25">
-      <c r="A5" s="42" t="str">
+      <c r="A5" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -6019,7 +6017,7 @@
       <c r="W5" s="2"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="str">
+      <c r="A6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>...A.01. - Tuberculosis</v>
       </c>
@@ -6077,7 +6075,7 @@
       <c r="W6" s="2"/>
     </row>
     <row r="7" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="str">
+      <c r="A7" s="16" t="str">
         <f t="shared" si="0"/>
         <v>...A.02. - HIV/ and other Sexually transmitted diseases (STDs)</v>
       </c>
@@ -6120,7 +6118,7 @@
       <c r="W7" s="2"/>
     </row>
     <row r="8" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="42" t="str">
+      <c r="A8" s="16" t="str">
         <f t="shared" si="0"/>
         <v>....A.02.a. - Sexually transmitted diseases (STDs) excluding HIV</v>
       </c>
@@ -6181,7 +6179,7 @@
       <c r="W8" s="2"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="42" t="str">
+      <c r="A9" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -6238,7 +6236,7 @@
       <c r="W9" s="2"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="42" t="str">
+      <c r="A10" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -6295,7 +6293,7 @@
       <c r="W10" s="2"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="42" t="str">
+      <c r="A11" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -6352,7 +6350,7 @@
       <c r="W11" s="2"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="42" t="str">
+      <c r="A12" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -6407,7 +6405,7 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="42" t="str">
+      <c r="A13" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -6464,7 +6462,7 @@
       <c r="W13" s="2"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="42" t="str">
+      <c r="A14" s="16" t="str">
         <f t="shared" si="0"/>
         <v>....A.02.b. - HIV/AIDS</v>
       </c>
@@ -6523,7 +6521,7 @@
       <c r="W14" s="2"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="42" t="str">
+      <c r="A15" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -6576,7 +6574,7 @@
       <c r="W15" s="2"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="42" t="str">
+      <c r="A16" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -6633,7 +6631,7 @@
       <c r="W16" s="2"/>
     </row>
     <row r="17" spans="1:23" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="42" t="str">
+      <c r="A17" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -6688,7 +6686,7 @@
       <c r="W17" s="2"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A18" s="42" t="str">
+      <c r="A18" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -6737,7 +6735,7 @@
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="42" t="str">
+      <c r="A19" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -6792,7 +6790,7 @@
       <c r="W19" s="2"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" s="42" t="str">
+      <c r="A20" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -6847,7 +6845,7 @@
       <c r="W20" s="2"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A21" s="42" t="str">
+      <c r="A21" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -6902,7 +6900,7 @@
       <c r="W21" s="2"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A22" s="42" t="str">
+      <c r="A22" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -6957,7 +6955,7 @@
       <c r="W22" s="2"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A23" s="42" t="str">
+      <c r="A23" s="16" t="str">
         <f t="shared" si="0"/>
         <v>...A.04. - Meningitis</v>
       </c>
@@ -7015,7 +7013,7 @@
       <c r="W23" s="2"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A24" s="42" t="str">
+      <c r="A24" s="16" t="str">
         <f t="shared" si="0"/>
         <v>...A.05. - Encephalitis</v>
       </c>
@@ -7073,7 +7071,7 @@
       <c r="W24" s="2"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A25" s="42" t="str">
+      <c r="A25" s="16" t="str">
         <f t="shared" si="0"/>
         <v>...A.06. - Hepatitis</v>
       </c>
@@ -7119,7 +7117,7 @@
       <c r="W25" s="2"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A26" s="42" t="str">
+      <c r="A26" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -7170,7 +7168,7 @@
       <c r="W26" s="2"/>
     </row>
     <row r="27" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="42" t="str">
+      <c r="A27" s="16" t="str">
         <f t="shared" si="0"/>
         <v>....A.06.a. - Acute hepatitis B</v>
       </c>
@@ -7226,7 +7224,7 @@
       <c r="W27" s="2"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A28" s="42" t="str">
+      <c r="A28" s="16" t="str">
         <f t="shared" si="0"/>
         <v>....A.06.b. - Acute hepatitis C</v>
       </c>
@@ -7282,7 +7280,7 @@
       <c r="W28" s="2"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A29" s="42" t="str">
+      <c r="A29" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -7333,7 +7331,7 @@
       <c r="W29" s="2"/>
     </row>
     <row r="30" spans="1:23" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="42" t="str">
+      <c r="A30" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -7381,7 +7379,7 @@
       <c r="W30" s="2"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A31" s="42" t="str">
+      <c r="A31" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -7436,7 +7434,7 @@
       <c r="W31" s="2"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A32" s="42" t="str">
+      <c r="A32" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -7491,7 +7489,7 @@
       <c r="W32" s="2"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A33" s="42" t="str">
+      <c r="A33" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -7546,7 +7544,7 @@
       <c r="W33" s="2"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A34" s="42" t="str">
+      <c r="A34" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -7601,7 +7599,7 @@
       <c r="W34" s="2"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A35" s="42" t="str">
+      <c r="A35" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -7656,7 +7654,7 @@
       <c r="W35" s="2"/>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A36" s="42" t="str">
+      <c r="A36" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -7707,7 +7705,7 @@
       <c r="W36" s="2"/>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A37" s="42" t="str">
+      <c r="A37" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -7758,7 +7756,7 @@
       <c r="W37" s="2"/>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A38" s="42" t="str">
+      <c r="A38" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -7813,7 +7811,7 @@
       <c r="W38" s="2"/>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A39" s="42" t="str">
+      <c r="A39" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -7868,7 +7866,7 @@
       <c r="W39" s="2"/>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A40" s="42" t="str">
+      <c r="A40" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -7919,7 +7917,7 @@
       <c r="W40" s="2"/>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A41" s="42" t="str">
+      <c r="A41" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -7974,7 +7972,7 @@
       <c r="W41" s="2"/>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A42" s="42" t="str">
+      <c r="A42" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -8025,7 +8023,7 @@
       <c r="W42" s="2"/>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A43" s="42" t="str">
+      <c r="A43" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -8080,7 +8078,7 @@
       <c r="W43" s="2"/>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A44" s="42" t="str">
+      <c r="A44" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -8135,7 +8133,7 @@
       <c r="W44" s="2"/>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A45" s="42" t="str">
+      <c r="A45" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -8187,7 +8185,7 @@
       <c r="W45" s="2"/>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A46" s="42" t="str">
+      <c r="A46" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -8242,7 +8240,7 @@
       <c r="W46" s="2"/>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A47" s="42" t="str">
+      <c r="A47" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -8293,7 +8291,7 @@
       <c r="W47" s="2"/>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A48" s="42" t="str">
+      <c r="A48" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -8344,7 +8342,7 @@
       <c r="W48" s="2"/>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A49" s="42" t="str">
+      <c r="A49" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -8395,7 +8393,7 @@
       <c r="W49" s="2"/>
     </row>
     <row r="50" spans="1:23" ht="102" x14ac:dyDescent="0.25">
-      <c r="A50" s="42" t="str">
+      <c r="A50" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -8458,7 +8456,7 @@
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A51" s="42" t="str">
+      <c r="A51" s="16" t="str">
         <f t="shared" si="0"/>
         <v>...A.07. - Respiratory infections</v>
       </c>
@@ -8515,7 +8513,7 @@
       <c r="W51" s="2"/>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A52" s="42" t="str">
+      <c r="A52" s="16" t="str">
         <f t="shared" si="0"/>
         <v>....A.07.a. - Lower respiratory infections</v>
       </c>
@@ -8581,7 +8579,7 @@
       <c r="W52" s="2"/>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A53" s="42" t="str">
+      <c r="A53" s="16" t="str">
         <f t="shared" si="0"/>
         <v>....A.07.b. - Upper respiratory infections</v>
       </c>
@@ -8647,7 +8645,7 @@
       <c r="W53" s="2"/>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A54" s="42" t="str">
+      <c r="A54" s="16" t="str">
         <f t="shared" si="0"/>
         <v>...A.10. - COVID-19</v>
       </c>
@@ -8691,7 +8689,7 @@
       <c r="W54" s="2"/>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A55" s="42" t="str">
+      <c r="A55" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -8752,7 +8750,7 @@
       <c r="W55" s="2"/>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A56" s="42" t="str">
+      <c r="A56" s="16" t="str">
         <f t="shared" si="0"/>
         <v>...A.08. - Maternal conditions</v>
       </c>
@@ -8811,7 +8809,7 @@
       <c r="W56" s="2"/>
     </row>
     <row r="57" spans="1:23" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A57" s="42" t="str">
+      <c r="A57" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -8874,7 +8872,7 @@
       </c>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A58" s="42" t="str">
+      <c r="A58" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -8935,7 +8933,7 @@
       <c r="W58" s="2"/>
     </row>
     <row r="59" spans="1:23" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A59" s="42" t="str">
+      <c r="A59" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -8998,7 +8996,7 @@
       </c>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A60" s="42" t="str">
+      <c r="A60" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -9059,7 +9057,7 @@
       <c r="W60" s="2"/>
     </row>
     <row r="61" spans="1:23" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A61" s="42" t="str">
+      <c r="A61" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -9120,7 +9118,7 @@
       <c r="W61" s="2"/>
     </row>
     <row r="62" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="42" t="str">
+      <c r="A62" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -9181,7 +9179,7 @@
       <c r="W62" s="2"/>
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A63" s="42" t="str">
+      <c r="A63" s="16" t="str">
         <f t="shared" si="0"/>
         <v>...A.09. - Neonatal conditions</v>
       </c>
@@ -9240,7 +9238,7 @@
       <c r="W63" s="2"/>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A64" s="42" t="str">
+      <c r="A64" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -9295,7 +9293,7 @@
       <c r="W64" s="2"/>
     </row>
     <row r="65" spans="1:23" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="42" t="str">
+      <c r="A65" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -9350,7 +9348,7 @@
       <c r="W65" s="2"/>
     </row>
     <row r="66" spans="1:23" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="42" t="str">
+      <c r="A66" s="16" t="str">
         <f t="shared" ref="A66:A126" si="6">IF(J66&lt;&gt;"",IF(H66&lt;&gt;"",CONCATENATE("....",F66,".",G66,".",H66,". - ",D66),IF(G66&lt;&gt;"",CONCATENATE("...",F66,".",G66,". - ",D66),CONCATENATE("..",F66,". - ",D66))),"")</f>
         <v/>
       </c>
@@ -9405,7 +9403,7 @@
       <c r="W66" s="2"/>
     </row>
     <row r="67" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="42" t="str">
+      <c r="A67" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -9466,7 +9464,7 @@
       <c r="W67" s="2"/>
     </row>
     <row r="68" spans="1:23" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="42" t="str">
+      <c r="A68" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -9518,7 +9516,7 @@
       <c r="W68" s="2"/>
     </row>
     <row r="69" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A69" s="42" t="str">
+      <c r="A69" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -9573,7 +9571,7 @@
       <c r="W69" s="2"/>
     </row>
     <row r="70" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A70" s="42" t="str">
+      <c r="A70" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -9628,7 +9626,7 @@
       <c r="W70" s="2"/>
     </row>
     <row r="71" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A71" s="42" t="str">
+      <c r="A71" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -9679,7 +9677,7 @@
       <c r="W71" s="2"/>
     </row>
     <row r="72" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A72" s="42" t="str">
+      <c r="A72" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -9734,7 +9732,7 @@
       <c r="W72" s="2"/>
     </row>
     <row r="73" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A73" s="42" t="str">
+      <c r="A73" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -9789,7 +9787,7 @@
       <c r="W73" s="2"/>
     </row>
     <row r="74" spans="1:23" ht="84" x14ac:dyDescent="0.25">
-      <c r="A74" s="42" t="str">
+      <c r="A74" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -9839,7 +9837,7 @@
       <c r="W74" s="2"/>
     </row>
     <row r="75" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A75" s="42" t="str">
+      <c r="A75" s="16" t="str">
         <f t="shared" si="6"/>
         <v>..D. - Other Chronic</v>
       </c>
@@ -9877,7 +9875,7 @@
       <c r="W75" s="2"/>
     </row>
     <row r="76" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="42" t="str">
+      <c r="A76" s="16" t="str">
         <f t="shared" si="6"/>
         <v>..B. - Cancer/Malignant neoplasms</v>
       </c>
@@ -9932,7 +9930,7 @@
       <c r="W76" s="2"/>
     </row>
     <row r="77" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A77" s="42" t="str">
+      <c r="A77" s="16" t="str">
         <f t="shared" si="6"/>
         <v>...B.01. - Mouth and oropharynx cancers</v>
       </c>
@@ -9988,7 +9986,7 @@
       <c r="W77" s="2"/>
     </row>
     <row r="78" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="42" t="str">
+      <c r="A78" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -10049,7 +10047,7 @@
       <c r="W78" s="2"/>
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A79" s="42" t="str">
+      <c r="A79" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -10110,7 +10108,7 @@
       <c r="W79" s="2"/>
     </row>
     <row r="80" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A80" s="42" t="str">
+      <c r="A80" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -10167,7 +10165,7 @@
       <c r="W80" s="2"/>
     </row>
     <row r="81" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A81" s="42" t="str">
+      <c r="A81" s="16" t="str">
         <f t="shared" si="6"/>
         <v>...B.02. - Esophagus cancer</v>
       </c>
@@ -10231,7 +10229,7 @@
       <c r="W81" s="2"/>
     </row>
     <row r="82" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A82" s="42" t="str">
+      <c r="A82" s="16" t="str">
         <f t="shared" si="6"/>
         <v>...B.03. - Stomach cancer</v>
       </c>
@@ -10297,7 +10295,7 @@
       </c>
     </row>
     <row r="83" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A83" s="42" t="str">
+      <c r="A83" s="16" t="str">
         <f t="shared" si="6"/>
         <v>...B.04. - Colon and rectum cancers</v>
       </c>
@@ -10361,7 +10359,7 @@
       <c r="W83" s="2"/>
     </row>
     <row r="84" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A84" s="42" t="str">
+      <c r="A84" s="16" t="str">
         <f t="shared" si="6"/>
         <v>...B.05. - Liver cancer</v>
       </c>
@@ -10425,7 +10423,7 @@
       <c r="W84" s="2"/>
     </row>
     <row r="85" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A85" s="42" t="str">
+      <c r="A85" s="16" t="str">
         <f t="shared" si="6"/>
         <v>...B.06. - Pancreas cancer</v>
       </c>
@@ -10489,7 +10487,7 @@
       <c r="W85" s="2"/>
     </row>
     <row r="86" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A86" s="42" t="str">
+      <c r="A86" s="16" t="str">
         <f t="shared" si="6"/>
         <v>...B.07. - Trachea, bronchus and lung cancers</v>
       </c>
@@ -10555,7 +10553,7 @@
       <c r="W86" s="2"/>
     </row>
     <row r="87" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A87" s="42" t="str">
+      <c r="A87" s="16" t="str">
         <f t="shared" si="6"/>
         <v>...B.08. - Melanoma and other skin cancers</v>
       </c>
@@ -10611,7 +10609,7 @@
       <c r="W87" s="2"/>
     </row>
     <row r="88" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="42" t="str">
+      <c r="A88" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -10672,7 +10670,7 @@
       <c r="W88" s="2"/>
     </row>
     <row r="89" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A89" s="42" t="str">
+      <c r="A89" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -10733,7 +10731,7 @@
       <c r="W89" s="2"/>
     </row>
     <row r="90" spans="1:23" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A90" s="42" t="str">
+      <c r="A90" s="16" t="str">
         <f t="shared" si="6"/>
         <v>...B.09. - Breast cancer</v>
       </c>
@@ -10797,7 +10795,7 @@
       <c r="W90" s="2"/>
     </row>
     <row r="91" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A91" s="42" t="str">
+      <c r="A91" s="16" t="str">
         <f t="shared" si="6"/>
         <v>...B.10. - Uterine cancer</v>
       </c>
@@ -10839,7 +10837,7 @@
       <c r="W91" s="2"/>
     </row>
     <row r="92" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A92" s="42" t="str">
+      <c r="A92" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -10900,7 +10898,7 @@
       <c r="W92" s="2"/>
     </row>
     <row r="93" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A93" s="42" t="str">
+      <c r="A93" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -10961,7 +10959,7 @@
       <c r="W93" s="2"/>
     </row>
     <row r="94" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A94" s="42" t="str">
+      <c r="A94" s="16" t="str">
         <f t="shared" si="6"/>
         <v>...B.11. - Ovary cancer</v>
       </c>
@@ -11025,7 +11023,7 @@
       <c r="W94" s="2"/>
     </row>
     <row r="95" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A95" s="42" t="str">
+      <c r="A95" s="16" t="str">
         <f t="shared" si="6"/>
         <v>...B.12. - Prostate cancer</v>
       </c>
@@ -11089,7 +11087,7 @@
       <c r="W95" s="2"/>
     </row>
     <row r="96" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A96" s="42" t="str">
+      <c r="A96" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -11150,7 +11148,7 @@
       <c r="W96" s="2"/>
     </row>
     <row r="97" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A97" s="42" t="str">
+      <c r="A97" s="16" t="str">
         <f t="shared" si="6"/>
         <v>...B.13. - Kidney, renal pelvis and ureter cancer</v>
       </c>
@@ -11214,7 +11212,7 @@
       <c r="W97" s="2"/>
     </row>
     <row r="98" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A98" s="42" t="str">
+      <c r="A98" s="16" t="str">
         <f t="shared" si="6"/>
         <v>...B.14. - Bladder cancer</v>
       </c>
@@ -11278,7 +11276,7 @@
       <c r="W98" s="2"/>
     </row>
     <row r="99" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A99" s="42" t="str">
+      <c r="A99" s="16" t="str">
         <f t="shared" si="6"/>
         <v>...B.15. - Brain and nervous system cancers</v>
       </c>
@@ -11342,7 +11340,7 @@
       <c r="W99" s="2"/>
     </row>
     <row r="100" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A100" s="42" t="str">
+      <c r="A100" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -11403,7 +11401,7 @@
       <c r="W100" s="2"/>
     </row>
     <row r="101" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A101" s="42" t="str">
+      <c r="A101" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -11464,7 +11462,7 @@
       <c r="W101" s="2"/>
     </row>
     <row r="102" spans="1:23" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A102" s="42" t="str">
+      <c r="A102" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -11525,7 +11523,7 @@
       <c r="W102" s="2"/>
     </row>
     <row r="103" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A103" s="42" t="str">
+      <c r="A103" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -11582,7 +11580,7 @@
       <c r="W103" s="2"/>
     </row>
     <row r="104" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A104" s="42" t="str">
+      <c r="A104" s="16" t="str">
         <f t="shared" si="6"/>
         <v>...B.16. - Lymphomas and multiple myeloma</v>
       </c>
@@ -11639,7 +11637,7 @@
       <c r="W104" s="2"/>
     </row>
     <row r="105" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A105" s="42" t="str">
+      <c r="A105" s="16" t="str">
         <f t="shared" si="6"/>
         <v>....B.16.a. - Hodgkin lymphoma</v>
       </c>
@@ -11701,7 +11699,7 @@
       <c r="W105" s="2"/>
     </row>
     <row r="106" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A106" s="42" t="str">
+      <c r="A106" s="16" t="str">
         <f t="shared" si="6"/>
         <v>....B.16.b. - Non-Hodgkin lymphoma</v>
       </c>
@@ -11763,7 +11761,7 @@
       <c r="W106" s="2"/>
     </row>
     <row r="107" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A107" s="42" t="str">
+      <c r="A107" s="16" t="str">
         <f t="shared" si="6"/>
         <v>....B.16.c. - Multiple myeloma</v>
       </c>
@@ -11825,7 +11823,7 @@
       <c r="W107" s="2"/>
     </row>
     <row r="108" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A108" s="42" t="str">
+      <c r="A108" s="16" t="str">
         <f t="shared" si="6"/>
         <v>...B.17. - Leukemia</v>
       </c>
@@ -11885,7 +11883,7 @@
       <c r="W108" s="2"/>
     </row>
     <row r="109" spans="1:23" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A109" s="42" t="str">
+      <c r="A109" s="16" t="str">
         <f t="shared" si="6"/>
         <v>...B.99. - Other malignant neoplasms</v>
       </c>
@@ -11945,7 +11943,7 @@
       <c r="W109" s="2"/>
     </row>
     <row r="110" spans="1:23" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A110" s="42" t="str">
+      <c r="A110" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -12000,7 +11998,7 @@
       <c r="W110" s="2"/>
     </row>
     <row r="111" spans="1:23" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A111" s="42" t="str">
+      <c r="A111" s="16" t="str">
         <f t="shared" si="6"/>
         <v>...D.01. - Diabetes mellitus</v>
       </c>
@@ -12070,7 +12068,7 @@
       </c>
     </row>
     <row r="112" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A112" s="42" t="str">
+      <c r="A112" s="16" t="str">
         <f t="shared" si="6"/>
         <v>...D.02. - Endocrine, blood, immune disorders</v>
       </c>
@@ -12129,7 +12127,7 @@
       <c r="W112" s="2"/>
     </row>
     <row r="113" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A113" s="42" t="str">
+      <c r="A113" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -12185,8 +12183,8 @@
       </c>
       <c r="W113" s="2"/>
     </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A114" s="42" t="str">
+    <row r="114" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A114" s="16" t="str">
         <f t="shared" si="6"/>
         <v>...D.03. - Sickle cell disorders and trait</v>
       </c>
@@ -12246,7 +12244,7 @@
       <c r="W114" s="2"/>
     </row>
     <row r="115" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A115" s="42" t="str">
+      <c r="A115" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -12303,7 +12301,7 @@
       <c r="W115" s="2"/>
     </row>
     <row r="116" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A116" s="42" t="str">
+      <c r="A116" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -12359,8 +12357,8 @@
       </c>
       <c r="W116" s="2"/>
     </row>
-    <row r="117" spans="1:23" ht="18" x14ac:dyDescent="0.25">
-      <c r="A117" s="42" t="str">
+    <row r="117" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A117" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -12416,7 +12414,7 @@
       <c r="W117" s="2"/>
     </row>
     <row r="118" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A118" s="42" t="str">
+      <c r="A118" s="16" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">...D.04. - Mental Health disorders </v>
       </c>
@@ -12459,7 +12457,7 @@
       <c r="W118" s="2"/>
     </row>
     <row r="119" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A119" s="42" t="str">
+      <c r="A119" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -12498,7 +12496,7 @@
       <c r="W119" s="2"/>
     </row>
     <row r="120" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A120" s="42" t="str">
+      <c r="A120" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -12528,7 +12526,7 @@
       <c r="W120" s="2"/>
     </row>
     <row r="121" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A121" s="42" t="str">
+      <c r="A121" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -12574,7 +12572,7 @@
       <c r="W121" s="2"/>
     </row>
     <row r="122" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A122" s="42" t="str">
+      <c r="A122" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -12633,7 +12631,7 @@
       <c r="W122" s="2"/>
     </row>
     <row r="123" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A123" s="42" t="str">
+      <c r="A123" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -12692,7 +12690,7 @@
       <c r="W123" s="2"/>
     </row>
     <row r="124" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A124" s="42" t="str">
+      <c r="A124" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -12751,7 +12749,7 @@
       <c r="W124" s="2"/>
     </row>
     <row r="125" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A125" s="42" t="str">
+      <c r="A125" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -12814,7 +12812,7 @@
       <c r="W125" s="2"/>
     </row>
     <row r="126" spans="1:23" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A126" s="42" t="str">
+      <c r="A126" s="16" t="str">
         <f t="shared" si="6"/>
         <v>....D.99.a. - Alcohol use disorders</v>
       </c>
@@ -12880,7 +12878,7 @@
       <c r="W126" s="2"/>
     </row>
     <row r="127" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A127" s="42" t="str">
+      <c r="A127" s="16" t="str">
         <f t="shared" ref="A127:A187" si="12">IF(J127&lt;&gt;"",IF(H127&lt;&gt;"",CONCATENATE("....",F127,".",G127,".",H127,". - ",D127),IF(G127&lt;&gt;"",CONCATENATE("...",F127,".",G127,". - ",D127),CONCATENATE("..",F127,". - ",D127))),"")</f>
         <v/>
       </c>
@@ -12935,7 +12933,7 @@
       <c r="W127" s="2"/>
     </row>
     <row r="128" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A128" s="42" t="str">
+      <c r="A128" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -12993,8 +12991,8 @@
       </c>
       <c r="W128" s="2"/>
     </row>
-    <row r="129" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A129" s="42" t="str">
+    <row r="129" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A129" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -13048,8 +13046,8 @@
       </c>
       <c r="W129" s="2"/>
     </row>
-    <row r="130" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A130" s="42" t="str">
+    <row r="130" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A130" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -13098,8 +13096,8 @@
       </c>
       <c r="W130" s="2"/>
     </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A131" s="42" t="str">
+    <row r="131" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A131" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -13154,7 +13152,7 @@
       <c r="W131" s="2"/>
     </row>
     <row r="132" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A132" s="42" t="str">
+      <c r="A132" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -13208,8 +13206,8 @@
       </c>
       <c r="W132" s="2"/>
     </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A133" s="42" t="str">
+    <row r="133" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A133" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -13263,8 +13261,8 @@
       </c>
       <c r="W133" s="2"/>
     </row>
-    <row r="134" spans="1:23" ht="33" x14ac:dyDescent="0.25">
-      <c r="A134" s="42" t="str">
+    <row r="134" spans="1:23" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A134" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -13319,7 +13317,7 @@
       <c r="W134" s="2"/>
     </row>
     <row r="135" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A135" s="42" t="str">
+      <c r="A135" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -13375,7 +13373,7 @@
       </c>
     </row>
     <row r="136" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A136" s="42" t="str">
+      <c r="A136" s="16" t="str">
         <f t="shared" si="12"/>
         <v>...D.06. - Alzheimer’s disease and other dementias</v>
       </c>
@@ -13437,7 +13435,7 @@
       <c r="W136" s="2"/>
     </row>
     <row r="137" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A137" s="42" t="str">
+      <c r="A137" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -13494,7 +13492,7 @@
       <c r="W137" s="2"/>
     </row>
     <row r="138" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A138" s="42" t="str">
+      <c r="A138" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -13551,7 +13549,7 @@
       <c r="W138" s="2"/>
     </row>
     <row r="139" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A139" s="42" t="str">
+      <c r="A139" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -13608,7 +13606,7 @@
       <c r="W139" s="2"/>
     </row>
     <row r="140" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A140" s="42" t="str">
+      <c r="A140" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -13661,7 +13659,7 @@
       <c r="W140" s="2"/>
     </row>
     <row r="141" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A141" s="42" t="str">
+      <c r="A141" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -13713,8 +13711,8 @@
       </c>
       <c r="W141" s="2"/>
     </row>
-    <row r="142" spans="1:23" ht="51" x14ac:dyDescent="0.25">
-      <c r="A142" s="42" t="str">
+    <row r="142" spans="1:23" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A142" s="16" t="str">
         <f t="shared" si="12"/>
         <v>...D.07. - Other neurological conditions</v>
       </c>
@@ -13778,7 +13776,7 @@
       <c r="W142" s="2"/>
     </row>
     <row r="143" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A143" s="42" t="str">
+      <c r="A143" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -13830,7 +13828,7 @@
       </c>
     </row>
     <row r="144" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A144" s="42" t="str">
+      <c r="A144" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -13883,7 +13881,7 @@
       <c r="W144" s="2"/>
     </row>
     <row r="145" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A145" s="42" t="str">
+      <c r="A145" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -13935,8 +13933,8 @@
       </c>
       <c r="W145" s="2"/>
     </row>
-    <row r="146" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A146" s="42" t="str">
+    <row r="146" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A146" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -13989,7 +13987,7 @@
       <c r="W146" s="2"/>
     </row>
     <row r="147" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A147" s="42" t="str">
+      <c r="A147" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -14042,7 +14040,7 @@
       <c r="W147" s="2"/>
     </row>
     <row r="148" spans="1:23" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A148" s="42" t="str">
+      <c r="A148" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -14095,7 +14093,7 @@
       <c r="W148" s="2"/>
     </row>
     <row r="149" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A149" s="42" t="str">
+      <c r="A149" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -14148,7 +14146,7 @@
       <c r="W149" s="2"/>
     </row>
     <row r="150" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A150" s="42" t="str">
+      <c r="A150" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -14203,7 +14201,7 @@
       </c>
     </row>
     <row r="151" spans="1:23" ht="42" x14ac:dyDescent="0.25">
-      <c r="A151" s="42" t="str">
+      <c r="A151" s="16" t="str">
         <f t="shared" si="12"/>
         <v>..C. - Cardiovascular diseases</v>
       </c>
@@ -14258,7 +14256,7 @@
       <c r="W151" s="2"/>
     </row>
     <row r="152" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A152" s="42" t="str">
+      <c r="A152" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -14319,7 +14317,7 @@
       <c r="W152" s="2"/>
     </row>
     <row r="153" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A153" s="42" t="str">
+      <c r="A153" s="16" t="str">
         <f t="shared" si="12"/>
         <v>...C.01. - Hypertensive heart disease</v>
       </c>
@@ -14383,7 +14381,7 @@
       <c r="W153" s="2"/>
     </row>
     <row r="154" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A154" s="42" t="str">
+      <c r="A154" s="16" t="str">
         <f t="shared" si="12"/>
         <v>...C.02. - Ischemic heart disease</v>
       </c>
@@ -14446,8 +14444,8 @@
       </c>
       <c r="W154" s="2"/>
     </row>
-    <row r="155" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A155" s="42" t="str">
+    <row r="155" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A155" s="16" t="str">
         <f t="shared" si="12"/>
         <v>...C.03. - Stroke</v>
       </c>
@@ -14515,7 +14513,7 @@
       <c r="W155" s="2"/>
     </row>
     <row r="156" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A156" s="42" t="str">
+      <c r="A156" s="16" t="str">
         <f t="shared" si="12"/>
         <v>...C.04. - Cardiomyopathy, myocarditis, endocarditis</v>
       </c>
@@ -14583,7 +14581,7 @@
       </c>
     </row>
     <row r="157" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A157" s="42" t="str">
+      <c r="A157" s="16" t="str">
         <f t="shared" si="12"/>
         <v>...C.05. -  Congestive heart failure</v>
       </c>
@@ -14635,7 +14633,7 @@
       <c r="W157" s="2"/>
     </row>
     <row r="158" spans="1:23" ht="51" x14ac:dyDescent="0.25">
-      <c r="A158" s="42" t="str">
+      <c r="A158" s="16" t="str">
         <f t="shared" si="12"/>
         <v>...C.99. - Other or unspecified cardiovascular diseases</v>
       </c>
@@ -14707,7 +14705,7 @@
       </c>
     </row>
     <row r="159" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A159" s="42" t="str">
+      <c r="A159" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -14761,7 +14759,7 @@
       <c r="W159" s="2"/>
     </row>
     <row r="160" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A160" s="42" t="str">
+      <c r="A160" s="16" t="str">
         <f t="shared" si="12"/>
         <v>...D.66. - Chronic obstructive pulmonary disease</v>
       </c>
@@ -14823,7 +14821,7 @@
       <c r="W160" s="2"/>
     </row>
     <row r="161" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A161" s="42" t="str">
+      <c r="A161" s="16" t="str">
         <f t="shared" si="12"/>
         <v>...D.67. - Asthma</v>
       </c>
@@ -14883,7 +14881,7 @@
       <c r="W161" s="2"/>
     </row>
     <row r="162" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A162" s="42" t="str">
+      <c r="A162" s="16" t="str">
         <f t="shared" si="12"/>
         <v>...D.68. - Other respiratory diseases</v>
       </c>
@@ -14943,7 +14941,7 @@
       <c r="W162" s="2"/>
     </row>
     <row r="163" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A163" s="42" t="str">
+      <c r="A163" s="16" t="str">
         <f t="shared" si="12"/>
         <v>...D.09. - Digestive diseases (excluding cirrhosis)</v>
       </c>
@@ -15006,7 +15004,7 @@
       <c r="W163" s="2"/>
     </row>
     <row r="164" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A164" s="42" t="str">
+      <c r="A164" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -15063,7 +15061,7 @@
       <c r="W164" s="2"/>
     </row>
     <row r="165" spans="1:23" s="46" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A165" s="42" t="str">
+      <c r="A165" s="16" t="str">
         <f t="shared" si="12"/>
         <v>...D.11. - Cirrhosis of the liver</v>
       </c>
@@ -15127,7 +15125,7 @@
       <c r="W165" s="2"/>
     </row>
     <row r="166" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A166" s="42" t="str">
+      <c r="A166" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -15184,7 +15182,7 @@
       <c r="W166" s="2"/>
     </row>
     <row r="167" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A167" s="42" t="str">
+      <c r="A167" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -15241,7 +15239,7 @@
       <c r="W167" s="2"/>
     </row>
     <row r="168" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A168" s="42" t="str">
+      <c r="A168" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -15298,7 +15296,7 @@
       <c r="W168" s="2"/>
     </row>
     <row r="169" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A169" s="42" t="str">
+      <c r="A169" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -15355,7 +15353,7 @@
       <c r="W169" s="2"/>
     </row>
     <row r="170" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A170" s="42" t="str">
+      <c r="A170" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -15412,7 +15410,7 @@
       <c r="W170" s="2"/>
     </row>
     <row r="171" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A171" s="42" t="str">
+      <c r="A171" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -15469,7 +15467,7 @@
       <c r="W171" s="2"/>
     </row>
     <row r="172" spans="1:23" ht="51" x14ac:dyDescent="0.25">
-      <c r="A172" s="42" t="str">
+      <c r="A172" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -15530,7 +15528,7 @@
       <c r="W172" s="2"/>
     </row>
     <row r="173" spans="1:23" ht="33" x14ac:dyDescent="0.25">
-      <c r="A173" s="42" t="str">
+      <c r="A173" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -15582,7 +15580,7 @@
       <c r="W173" s="2"/>
     </row>
     <row r="174" spans="1:23" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A174" s="42" t="str">
+      <c r="A174" s="16" t="str">
         <f t="shared" si="12"/>
         <v>...D.10. - Kidney diseases</v>
       </c>
@@ -15643,7 +15641,7 @@
       <c r="W174" s="2"/>
     </row>
     <row r="175" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A175" s="42" t="str">
+      <c r="A175" s="16" t="str">
         <f t="shared" si="12"/>
         <v>....D.10.a. - Acute glomerulonephritis</v>
       </c>
@@ -15707,7 +15705,7 @@
       <c r="W175" s="2"/>
     </row>
     <row r="176" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A176" s="42" t="str">
+      <c r="A176" s="16" t="str">
         <f t="shared" si="12"/>
         <v>....D.10.b. - Chronic kidney disease due to diabetes</v>
       </c>
@@ -15771,7 +15769,7 @@
       <c r="W176" s="2"/>
     </row>
     <row r="177" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A177" s="42" t="str">
+      <c r="A177" s="16" t="str">
         <f t="shared" si="12"/>
         <v>....D.10.c. - Other chronic kidney disease</v>
       </c>
@@ -15835,7 +15833,7 @@
       <c r="W177" s="2"/>
     </row>
     <row r="178" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A178" s="42" t="str">
+      <c r="A178" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -15888,7 +15886,7 @@
       <c r="W178" s="2"/>
     </row>
     <row r="179" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A179" s="42" t="str">
+      <c r="A179" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -15945,7 +15943,7 @@
       <c r="W179" s="2"/>
     </row>
     <row r="180" spans="1:23" ht="24" x14ac:dyDescent="0.25">
-      <c r="A180" s="42" t="str">
+      <c r="A180" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -16002,7 +16000,7 @@
       <c r="W180" s="2"/>
     </row>
     <row r="181" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A181" s="42" t="str">
+      <c r="A181" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -16059,7 +16057,7 @@
       <c r="W181" s="2"/>
     </row>
     <row r="182" spans="1:23" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A182" s="42" t="str">
+      <c r="A182" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -16116,7 +16114,7 @@
       <c r="W182" s="2"/>
     </row>
     <row r="183" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A183" s="42" t="str">
+      <c r="A183" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -16171,7 +16169,7 @@
       <c r="W183" s="2"/>
     </row>
     <row r="184" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A184" s="42" t="str">
+      <c r="A184" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -16227,7 +16225,7 @@
       <c r="W184" s="2"/>
     </row>
     <row r="185" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A185" s="42" t="str">
+      <c r="A185" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -16284,7 +16282,7 @@
       <c r="W185" s="2"/>
     </row>
     <row r="186" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A186" s="42" t="str">
+      <c r="A186" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -16337,7 +16335,7 @@
       <c r="W186" s="2"/>
     </row>
     <row r="187" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A187" s="42" t="str">
+      <c r="A187" s="16" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -16390,7 +16388,7 @@
       <c r="W187" s="2"/>
     </row>
     <row r="188" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A188" s="42" t="str">
+      <c r="A188" s="16" t="str">
         <f t="shared" ref="A188:A232" si="20">IF(J188&lt;&gt;"",IF(H188&lt;&gt;"",CONCATENATE("....",F188,".",G188,".",H188,". - ",D188),IF(G188&lt;&gt;"",CONCATENATE("...",F188,".",G188,". - ",D188),CONCATENATE("..",F188,". - ",D188))),"")</f>
         <v/>
       </c>
@@ -16443,7 +16441,7 @@
       <c r="W188" s="2"/>
     </row>
     <row r="189" spans="1:23" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A189" s="42" t="str">
+      <c r="A189" s="16" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
@@ -16504,7 +16502,7 @@
       <c r="W189" s="2"/>
     </row>
     <row r="190" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A190" s="42" t="str">
+      <c r="A190" s="16" t="str">
         <f t="shared" si="20"/>
         <v>...D.12. - Congenital anomalies</v>
       </c>
@@ -16563,7 +16561,7 @@
       <c r="W190" s="2"/>
     </row>
     <row r="191" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A191" s="42" t="str">
+      <c r="A191" s="16" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
@@ -16620,7 +16618,7 @@
       <c r="W191" s="2"/>
     </row>
     <row r="192" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A192" s="42" t="str">
+      <c r="A192" s="16" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
@@ -16677,7 +16675,7 @@
       <c r="W192" s="2"/>
     </row>
     <row r="193" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A193" s="42" t="str">
+      <c r="A193" s="16" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
@@ -16734,7 +16732,7 @@
       <c r="W193" s="2"/>
     </row>
     <row r="194" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A194" s="42" t="str">
+      <c r="A194" s="16" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
@@ -16791,7 +16789,7 @@
       <c r="W194" s="2"/>
     </row>
     <row r="195" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A195" s="42" t="str">
+      <c r="A195" s="16" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
@@ -16848,7 +16846,7 @@
       <c r="W195" s="2"/>
     </row>
     <row r="196" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A196" s="42" t="str">
+      <c r="A196" s="16" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
@@ -16905,7 +16903,7 @@
       <c r="W196" s="2"/>
     </row>
     <row r="197" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A197" s="42" t="str">
+      <c r="A197" s="16" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
@@ -16955,7 +16953,7 @@
       <c r="W197" s="2"/>
     </row>
     <row r="198" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A198" s="42" t="str">
+      <c r="A198" s="16" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
@@ -17008,7 +17006,7 @@
       <c r="W198" s="2"/>
     </row>
     <row r="199" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A199" s="42" t="str">
+      <c r="A199" s="16" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
@@ -17061,7 +17059,7 @@
       <c r="W199" s="2"/>
     </row>
     <row r="200" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A200" s="42" t="str">
+      <c r="A200" s="16" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
@@ -17114,7 +17112,7 @@
       <c r="W200" s="2"/>
     </row>
     <row r="201" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A201" s="42" t="str">
+      <c r="A201" s="16" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
@@ -17167,7 +17165,7 @@
       <c r="W201" s="2"/>
     </row>
     <row r="202" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A202" s="42" t="str">
+      <c r="A202" s="16" t="str">
         <f>IF(J202&lt;&gt;"",IF(H202&lt;&gt;"",CONCATENATE("....",F202,".",G202,".",H202,". - ",D202),IF(G202&lt;&gt;"",CONCATENATE("...",F202,".",G202,". - ",D202),CONCATENATE("..",F202,". - ",D202))),"")</f>
         <v>...D.99. - Other Chronic Conditions</v>
       </c>
@@ -17187,7 +17185,7 @@
       </c>
     </row>
     <row r="203" spans="1:23" ht="24" x14ac:dyDescent="0.25">
-      <c r="A203" s="42" t="str">
+      <c r="A203" s="16" t="str">
         <f t="shared" si="20"/>
         <v>..E. - Injuries</v>
       </c>
@@ -17242,7 +17240,7 @@
       <c r="W203" s="2"/>
     </row>
     <row r="204" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A204" s="42" t="str">
+      <c r="A204" s="16" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
@@ -17296,7 +17294,7 @@
       <c r="W204" s="2"/>
     </row>
     <row r="205" spans="1:23" ht="36" x14ac:dyDescent="0.25">
-      <c r="A205" s="42" t="str">
+      <c r="A205" s="16" t="str">
         <f t="shared" si="20"/>
         <v>...E.01. - Road injury</v>
       </c>
@@ -17360,7 +17358,7 @@
       <c r="W205" s="2"/>
     </row>
     <row r="206" spans="1:23" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A206" s="42" t="str">
+      <c r="A206" s="16" t="str">
         <f t="shared" si="20"/>
         <v>...E.02. - Drug overdose (poisoning/substance use disorders)</v>
       </c>
@@ -17410,7 +17408,7 @@
       <c r="W206" s="2"/>
     </row>
     <row r="207" spans="1:23" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A207" s="42" t="str">
+      <c r="A207" s="16" t="str">
         <f t="shared" ref="A207:A212" si="24">IF(J207&lt;&gt;"",IF(H207&lt;&gt;"",CONCATENATE("....",F207,".",G207,".",H207,". - ",D207),IF(G207&lt;&gt;"",CONCATENATE("...",F207,".",G207,". - ",D207),CONCATENATE("..",F207,". - ",D207))),"")</f>
         <v/>
       </c>
@@ -17460,7 +17458,7 @@
       <c r="W207" s="2"/>
     </row>
     <row r="208" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A208" s="42" t="str">
+      <c r="A208" s="16" t="str">
         <f t="shared" si="24"/>
         <v/>
       </c>
@@ -17517,7 +17515,7 @@
       <c r="W208" s="2"/>
     </row>
     <row r="209" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A209" s="42" t="str">
+      <c r="A209" s="16" t="str">
         <f t="shared" si="24"/>
         <v/>
       </c>
@@ -17574,7 +17572,7 @@
       <c r="W209" s="2"/>
     </row>
     <row r="210" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A210" s="42" t="str">
+      <c r="A210" s="16" t="str">
         <f t="shared" si="24"/>
         <v/>
       </c>
@@ -17626,7 +17624,7 @@
       <c r="W210" s="2"/>
     </row>
     <row r="211" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A211" s="42" t="str">
+      <c r="A211" s="16" t="str">
         <f t="shared" si="24"/>
         <v/>
       </c>
@@ -17683,7 +17681,7 @@
       <c r="W211" s="2"/>
     </row>
     <row r="212" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A212" s="42" t="str">
+      <c r="A212" s="16" t="str">
         <f t="shared" si="24"/>
         <v/>
       </c>
@@ -17746,7 +17744,7 @@
       </c>
     </row>
     <row r="213" spans="1:23" ht="51" x14ac:dyDescent="0.25">
-      <c r="A213" s="42" t="str">
+      <c r="A213" s="16" t="str">
         <f t="shared" si="20"/>
         <v>...E.03. - Poisonings (non-drug)</v>
       </c>
@@ -17808,7 +17806,7 @@
       <c r="W213" s="2"/>
     </row>
     <row r="214" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A214" s="42" t="str">
+      <c r="A214" s="16" t="str">
         <f t="shared" si="20"/>
         <v>...E.04. - Falls</v>
       </c>
@@ -17870,7 +17868,7 @@
       <c r="W214" s="2"/>
     </row>
     <row r="215" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A215" s="42" t="str">
+      <c r="A215" s="16" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
@@ -17925,7 +17923,7 @@
       <c r="W215" s="2"/>
     </row>
     <row r="216" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A216" s="42" t="str">
+      <c r="A216" s="16" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
@@ -17982,7 +17980,7 @@
       <c r="W216" s="2"/>
     </row>
     <row r="217" spans="1:23" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A217" s="42" t="str">
+      <c r="A217" s="16" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
@@ -18039,7 +18037,7 @@
       <c r="W217" s="2"/>
     </row>
     <row r="218" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A218" s="42" t="str">
+      <c r="A218" s="16" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
@@ -18086,7 +18084,7 @@
       <c r="W218" s="2"/>
     </row>
     <row r="219" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A219" s="42" t="str">
+      <c r="A219" s="16" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
@@ -18143,7 +18141,7 @@
       <c r="W219" s="2"/>
     </row>
     <row r="220" spans="1:23" ht="51" x14ac:dyDescent="0.25">
-      <c r="A220" s="42" t="str">
+      <c r="A220" s="16" t="str">
         <f t="shared" si="20"/>
         <v>...E.05. - Other unintentional injuries</v>
       </c>
@@ -18209,7 +18207,7 @@
       </c>
     </row>
     <row r="221" spans="1:23" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A221" s="42" t="str">
+      <c r="A221" s="16" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
@@ -18259,7 +18257,7 @@
       <c r="W221" s="2"/>
     </row>
     <row r="222" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A222" s="42" t="str">
+      <c r="A222" s="16" t="str">
         <f t="shared" si="20"/>
         <v>...E.07. - Suicide/Self-harm</v>
       </c>
@@ -18323,7 +18321,7 @@
       <c r="W222" s="2"/>
     </row>
     <row r="223" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A223" s="42" t="str">
+      <c r="A223" s="16" t="str">
         <f t="shared" si="20"/>
         <v>...E.08. - Homicide/Interpersonal violence</v>
       </c>
@@ -18380,7 +18378,7 @@
       <c r="W223" s="2"/>
     </row>
     <row r="224" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A224" s="42" t="str">
+      <c r="A224" s="16" t="str">
         <f t="shared" si="20"/>
         <v>....E.08.a. - Homicide excluding legal intervention</v>
       </c>
@@ -18428,7 +18426,7 @@
       <c r="W224" s="2"/>
     </row>
     <row r="225" spans="1:23" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A225" s="42" t="str">
+      <c r="A225" s="16" t="str">
         <f t="shared" si="20"/>
         <v>....E.08.b. - Legal intervention</v>
       </c>
@@ -18478,7 +18476,7 @@
       <c r="W225" s="2"/>
     </row>
     <row r="226" spans="1:23" ht="102" x14ac:dyDescent="0.25">
-      <c r="A226" s="42" t="str">
+      <c r="A226" s="16" t="str">
         <f t="shared" si="20"/>
         <v>....E.08.c. - Execution, War, Terrorism</v>
       </c>
@@ -18542,7 +18540,7 @@
       </c>
     </row>
     <row r="227" spans="1:23" ht="51" x14ac:dyDescent="0.25">
-      <c r="A227" s="42" t="str">
+      <c r="A227" s="16" t="str">
         <f t="shared" si="20"/>
         <v>...E.99. - Injuries of unknown intent (e.g., unintentional or self-harm), including overdoses and deaths by firearm</v>
       </c>
@@ -18584,7 +18582,7 @@
       </c>
     </row>
     <row r="228" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A228" s="42" t="str">
+      <c r="A228" s="16" t="str">
         <f t="shared" si="20"/>
         <v>...Z.01. - Symptoms, signs and ill-defined conditions, not elsewhere classified</v>
       </c>
@@ -18622,7 +18620,7 @@
       </c>
     </row>
     <row r="229" spans="1:23" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A229" s="42" t="str">
+      <c r="A229" s="16" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
@@ -18654,7 +18652,7 @@
       </c>
     </row>
     <row r="230" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A230" s="42" t="str">
+      <c r="A230" s="16" t="str">
         <f t="shared" si="20"/>
         <v>...Z.02. - Unknown/Missing Value</v>
       </c>
@@ -18674,7 +18672,7 @@
       </c>
     </row>
     <row r="231" spans="1:23" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A231" s="42" t="str">
+      <c r="A231" s="16" t="str">
         <f t="shared" si="20"/>
         <v>...Z.03. - Code does not map</v>
       </c>
@@ -18697,7 +18695,7 @@
       </c>
     </row>
     <row r="232" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A232" s="42" t="str">
+      <c r="A232" s="16" t="str">
         <f t="shared" si="20"/>
         <v>..Z. - Unknown/Missing Value</v>
       </c>

</xml_diff>

<commit_message>
Add detailedRace to xMDA
</commit_message>
<xml_diff>
--- a/myCCB/myInfo/icd10_to_CAUSE.xlsx
+++ b/myCCB/myInfo/icd10_to_CAUSE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB\myCCB\myInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2313FF37-958B-4FC5-9A9D-906051281104}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D75FD0-CC05-48BE-AE63-C6B1B1D69241}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -4255,9 +4255,6 @@
     <t>U010-U019, U02, X85-Y09, Y871</t>
   </si>
   <si>
-    <t>Y355,  Y36, Y891, Y38, y899</t>
-  </si>
-  <si>
     <t>Y355|Y36|Y37|Y891|Y38</t>
   </si>
   <si>
@@ -4737,6 +4734,9 @@
   </si>
   <si>
     <t>U07[1-2]</t>
+  </si>
+  <si>
+    <t>Y355,  Y36, Y891, Y38</t>
   </si>
 </sst>
 </file>
@@ -5772,10 +5772,10 @@
   <dimension ref="A1:W238"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="K125" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K62" sqref="K62"/>
+      <selection pane="bottomRight" activeCell="A159" sqref="A159:XFD159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="49" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5815,13 +5815,13 @@
         <v>762</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>1400</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>1401</v>
       </c>
-      <c r="E1" s="21" t="s">
-        <v>1402</v>
-      </c>
       <c r="F1" s="23" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="G1" s="24" t="s">
         <v>1119</v>
@@ -5833,7 +5833,7 @@
         <v>1121</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>1292</v>
@@ -5979,10 +5979,10 @@
         <v>1125</v>
       </c>
       <c r="D4" s="20" t="s">
+        <v>1433</v>
+      </c>
+      <c r="E4" s="20" t="s">
         <v>1434</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>1435</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>1131</v>
@@ -6131,7 +6131,7 @@
         <v>1147</v>
       </c>
       <c r="E7" s="71" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>1131</v>
@@ -6348,7 +6348,7 @@
         <v>6</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E11" s="71"/>
       <c r="F11" s="6" t="s">
@@ -6686,7 +6686,7 @@
         <v>10</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="E17" s="71"/>
       <c r="F17" s="6" t="s">
@@ -7246,10 +7246,10 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5" t="s">
+        <v>1397</v>
+      </c>
+      <c r="N27" s="16" t="s">
         <v>1398</v>
-      </c>
-      <c r="N27" s="16" t="s">
-        <v>1399</v>
       </c>
       <c r="Q27" s="55" t="s">
         <v>960</v>
@@ -8397,7 +8397,7 @@
         <v>696</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="E49" s="71"/>
       <c r="F49" s="6" t="s">
@@ -8473,7 +8473,7 @@
         <v>1217</v>
       </c>
       <c r="N50" s="19" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="O50" s="19"/>
       <c r="P50" s="19"/>
@@ -8520,7 +8520,7 @@
       <c r="I51" s="38"/>
       <c r="J51" s="38"/>
       <c r="K51" s="5" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="L51" s="5"/>
       <c r="M51" s="5" t="s">
@@ -8575,7 +8575,7 @@
         <v/>
       </c>
       <c r="K52" s="5" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="L52" s="5"/>
       <c r="M52" s="5" t="s">
@@ -8634,7 +8634,7 @@
         <v/>
       </c>
       <c r="K53" s="5" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="L53" s="5"/>
       <c r="M53" s="5" t="s">
@@ -8676,10 +8676,10 @@
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="33" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="E54" s="71"/>
       <c r="F54" s="6" t="s">
@@ -8700,10 +8700,10 @@
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
       <c r="M54" s="5" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="N54" s="5" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="O54" s="5"/>
       <c r="P54" s="5"/>
@@ -8722,10 +8722,10 @@
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="33" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="E55" s="71"/>
       <c r="F55" s="6" t="s">
@@ -8746,10 +8746,10 @@
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
       <c r="M55" s="5" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="N55" s="5" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="O55" s="5"/>
       <c r="P55" s="5"/>
@@ -8768,10 +8768,10 @@
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="33" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="E56" s="71"/>
       <c r="F56" s="6" t="s">
@@ -8792,10 +8792,10 @@
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
       <c r="M56" s="5" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="N56" s="16" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="Q56" s="55"/>
       <c r="R56" s="56"/>
@@ -8812,13 +8812,13 @@
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="30" t="s">
+        <v>1469</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>1469</v>
+      </c>
+      <c r="E57" s="71" t="s">
         <v>1470</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>1470</v>
-      </c>
-      <c r="E57" s="71" t="s">
-        <v>1471</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>1131</v>
@@ -8833,14 +8833,14 @@
       </c>
       <c r="J57" s="38"/>
       <c r="K57" s="5" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="L57" s="5"/>
       <c r="M57" s="5" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="N57" s="5" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="O57" s="5"/>
       <c r="P57" s="5"/>
@@ -8880,7 +8880,7 @@
       </c>
       <c r="J58" s="38"/>
       <c r="K58" s="5" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="L58" s="5"/>
       <c r="M58" s="5" t="s">
@@ -8986,7 +8986,7 @@
         <v>33</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="E60" s="71"/>
       <c r="F60" s="6" t="s">
@@ -9173,7 +9173,7 @@
         <v>36</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="E63" s="71"/>
       <c r="F63" s="6" t="s">
@@ -9461,7 +9461,7 @@
     <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
       <c r="C68" s="30" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="71"/>
@@ -9479,13 +9479,13 @@
       <c r="J68" s="38"/>
       <c r="K68" s="5"/>
       <c r="L68" s="5" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="M68" s="5" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="N68" s="16" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="Q68" s="55"/>
       <c r="R68" s="56"/>
@@ -9891,7 +9891,7 @@
         <v>48</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="E76" s="71"/>
       <c r="F76" s="6" t="s">
@@ -10026,7 +10026,7 @@
         <v>383</v>
       </c>
       <c r="S78" s="68" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="T78" s="65" t="s">
         <v>557</v>
@@ -10261,7 +10261,7 @@
         <v>699</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="E83" s="71"/>
       <c r="F83" s="6" t="s">
@@ -10379,7 +10379,7 @@
         <v>53</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="E85" s="74"/>
       <c r="F85" s="6" t="s">
@@ -10704,7 +10704,7 @@
         <v>221</v>
       </c>
       <c r="E90" s="74" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="F90" s="6" t="s">
         <v>1132</v>
@@ -10964,16 +10964,16 @@
         <v>B09</v>
       </c>
       <c r="K94" s="16" t="s">
+        <v>1461</v>
+      </c>
+      <c r="L94" s="18" t="s">
         <v>1462</v>
       </c>
-      <c r="L94" s="18" t="s">
+      <c r="M94" s="5" t="s">
         <v>1463</v>
       </c>
-      <c r="M94" s="5" t="s">
+      <c r="N94" s="47" t="s">
         <v>1464</v>
-      </c>
-      <c r="N94" s="47" t="s">
-        <v>1465</v>
       </c>
       <c r="O94" s="47"/>
       <c r="P94" s="47"/>
@@ -11554,7 +11554,7 @@
         <v>707</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="E104" s="71"/>
       <c r="F104" s="6" t="s">
@@ -11692,16 +11692,16 @@
       </c>
       <c r="J106" s="38"/>
       <c r="K106" s="19" t="s">
+        <v>1457</v>
+      </c>
+      <c r="L106" s="18" t="s">
         <v>1458</v>
       </c>
-      <c r="L106" s="18" t="s">
+      <c r="M106" s="5" t="s">
         <v>1459</v>
       </c>
-      <c r="M106" s="5" t="s">
+      <c r="N106" s="47" t="s">
         <v>1460</v>
-      </c>
-      <c r="N106" s="47" t="s">
-        <v>1461</v>
       </c>
       <c r="O106" s="47"/>
       <c r="P106" s="47"/>
@@ -12037,7 +12037,7 @@
         <v>715</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="E112" s="71"/>
       <c r="F112" s="6" t="s">
@@ -12458,7 +12458,7 @@
         <v>719</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="E119" s="71"/>
       <c r="F119" s="6" t="s">
@@ -12666,10 +12666,10 @@
       </c>
       <c r="B123" s="2"/>
       <c r="C123" s="31" t="s">
+        <v>1359</v>
+      </c>
+      <c r="D123" s="2" t="s">
         <v>1360</v>
-      </c>
-      <c r="D123" s="2" t="s">
-        <v>1361</v>
       </c>
       <c r="E123" s="71"/>
       <c r="F123" s="6"/>
@@ -12681,7 +12681,7 @@
         <v/>
       </c>
       <c r="K123" s="77" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="L123" s="5"/>
       <c r="M123" s="5"/>
@@ -12973,7 +12973,7 @@
         <v>1139</v>
       </c>
       <c r="H129" s="6" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="I129" s="38" t="str">
         <f>CONCATENATE("c",F129,G129,H129)</f>
@@ -13102,7 +13102,7 @@
         <v>1139</v>
       </c>
       <c r="H131" s="6" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="I131" s="38" t="str">
         <f t="shared" ref="I131:I133" si="14">CONCATENATE("c",F131,G131,H131)</f>
@@ -13157,7 +13157,7 @@
         <v>1139</v>
       </c>
       <c r="H132" s="6" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="I132" s="38" t="str">
         <f t="shared" si="14"/>
@@ -13206,7 +13206,7 @@
         <v>729</v>
       </c>
       <c r="D133" s="5" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="E133" s="74"/>
       <c r="F133" s="6" t="s">
@@ -13216,7 +13216,7 @@
         <v>1139</v>
       </c>
       <c r="H133" s="6" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="I133" s="38" t="str">
         <f t="shared" si="14"/>
@@ -13261,7 +13261,7 @@
         <v>74</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="E134" s="74"/>
       <c r="F134" s="6"/>
@@ -13321,7 +13321,7 @@
         <v>1139</v>
       </c>
       <c r="H135" s="6" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="I135" s="38" t="str">
         <f>CONCATENATE("c",F135,G135,H135)</f>
@@ -13376,7 +13376,7 @@
         <v>1139</v>
       </c>
       <c r="H136" s="6" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="I136" s="38" t="str">
         <f>CONCATENATE("c",F136,G136,H136)</f>
@@ -13431,7 +13431,7 @@
         <v>1139</v>
       </c>
       <c r="H137" s="6" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="I137" s="38" t="str">
         <f>CONCATENATE("c",F137,G137,H137)</f>
@@ -13476,7 +13476,7 @@
         <v>76</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="E138" s="71"/>
       <c r="F138" s="6" t="s">
@@ -13486,7 +13486,7 @@
         <v>1139</v>
       </c>
       <c r="H138" s="6" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="I138" s="38" t="str">
         <f>CONCATENATE("c",F138,G138,H138)</f>
@@ -13590,7 +13590,7 @@
         <v>255</v>
       </c>
       <c r="E140" s="71" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="F140" s="6" t="s">
         <v>1134</v>
@@ -14275,7 +14275,7 @@
         <v>460</v>
       </c>
       <c r="N152" s="47" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="O152" s="47"/>
       <c r="P152" s="47"/>
@@ -14595,7 +14595,7 @@
         <v>96</v>
       </c>
       <c r="D158" s="5" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="E158" s="74"/>
       <c r="F158" s="6" t="s">
@@ -14730,7 +14730,7 @@
         <v>275</v>
       </c>
       <c r="E160" s="74" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F160" s="6" t="s">
         <v>1133</v>
@@ -14791,7 +14791,7 @@
       <c r="B161" s="2"/>
       <c r="C161" s="34"/>
       <c r="D161" s="5" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="E161" s="74"/>
       <c r="F161" s="6" t="s">
@@ -14850,7 +14850,7 @@
         <v>1298</v>
       </c>
       <c r="E162" s="71" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="F162" s="6" t="s">
         <v>1133</v>
@@ -14868,7 +14868,7 @@
         <v>C99</v>
       </c>
       <c r="K162" s="5" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="L162" s="5" t="s">
         <v>1300</v>
@@ -14976,7 +14976,7 @@
         <v>278</v>
       </c>
       <c r="E164" s="71" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="F164" s="6" t="s">
         <v>1134</v>
@@ -15158,7 +15158,7 @@
         <v>1305</v>
       </c>
       <c r="E167" s="71" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="F167" s="6" t="s">
         <v>1134</v>
@@ -15175,7 +15175,7 @@
         <v>D09</v>
       </c>
       <c r="K167" s="62" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="L167" s="5"/>
       <c r="M167" s="5" t="s">
@@ -15303,7 +15303,7 @@
         <v>1189</v>
       </c>
       <c r="N169" s="47" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="O169" s="47"/>
       <c r="P169" s="47"/>
@@ -15919,7 +15919,7 @@
         <v>740</v>
       </c>
       <c r="D180" s="5" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="E180" s="71"/>
       <c r="F180" s="6" t="s">
@@ -16347,7 +16347,7 @@
         <v>483</v>
       </c>
       <c r="N187" s="47" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="O187" s="47"/>
       <c r="P187" s="47"/>
@@ -17429,7 +17429,7 @@
         <v>1113</v>
       </c>
       <c r="S207" s="68" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="T207" s="65" t="s">
         <v>654</v>
@@ -17567,13 +17567,13 @@
       </c>
       <c r="B210" s="2"/>
       <c r="C210" s="30" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="D210" s="5" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="E210" s="71" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="F210" s="6" t="s">
         <v>1135</v>
@@ -17591,14 +17591,14 @@
         <v>E02</v>
       </c>
       <c r="K210" s="76" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="L210" s="5"/>
       <c r="M210" s="5" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="N210" s="19" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="O210" s="19"/>
       <c r="P210" s="19"/>
@@ -17690,10 +17690,10 @@
       <c r="K212" s="5"/>
       <c r="L212" s="5"/>
       <c r="M212" s="5" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="N212" s="47" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="O212" s="47"/>
       <c r="P212" s="47"/>
@@ -17838,7 +17838,7 @@
         <v>726</v>
       </c>
       <c r="D215" s="5" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="E215" s="71"/>
       <c r="F215" s="6" t="s">
@@ -17911,16 +17911,16 @@
       </c>
       <c r="J216" s="38"/>
       <c r="K216" s="5" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="L216" s="5" t="s">
         <v>1152</v>
       </c>
       <c r="M216" s="5" t="s">
+        <v>1357</v>
+      </c>
+      <c r="N216" s="19" t="s">
         <v>1358</v>
-      </c>
-      <c r="N216" s="19" t="s">
-        <v>1359</v>
       </c>
       <c r="O216" s="19"/>
       <c r="P216" s="19"/>
@@ -17955,10 +17955,10 @@
         <v>200</v>
       </c>
       <c r="C217" s="30" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="D217" s="5" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="E217" s="71"/>
       <c r="F217" s="6" t="s">
@@ -17978,13 +17978,13 @@
       </c>
       <c r="K217" s="5"/>
       <c r="L217" s="5" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="M217" s="5" t="s">
+        <v>1371</v>
+      </c>
+      <c r="N217" s="47" t="s">
         <v>1372</v>
-      </c>
-      <c r="N217" s="47" t="s">
-        <v>1373</v>
       </c>
       <c r="O217" s="47"/>
       <c r="P217" s="47"/>
@@ -18212,10 +18212,10 @@
       <c r="K221" s="5"/>
       <c r="L221" s="5"/>
       <c r="M221" s="5" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="N221" s="47" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="O221" s="47"/>
       <c r="P221" s="47"/>
@@ -18246,10 +18246,10 @@
       </c>
       <c r="B222" s="2"/>
       <c r="C222" s="30" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="D222" s="5" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="E222" s="71"/>
       <c r="F222" s="6" t="s">
@@ -18265,16 +18265,16 @@
       </c>
       <c r="J222" s="38"/>
       <c r="K222" s="5" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="L222" s="5" t="s">
         <v>1199</v>
       </c>
       <c r="M222" s="5" t="s">
+        <v>1347</v>
+      </c>
+      <c r="N222" s="47" t="s">
         <v>1348</v>
-      </c>
-      <c r="N222" s="47" t="s">
-        <v>1349</v>
       </c>
       <c r="O222" s="47"/>
       <c r="P222" s="47"/>
@@ -18374,7 +18374,7 @@
         <v>E05</v>
       </c>
       <c r="K224" s="5" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="L224" s="5" t="s">
         <v>1238</v>
@@ -18538,7 +18538,7 @@
         <v>1257</v>
       </c>
       <c r="E227" s="71" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="F227" s="6" t="s">
         <v>1135</v>
@@ -18609,14 +18609,14 @@
         <v>E08a</v>
       </c>
       <c r="K228" s="5" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="L228" s="5"/>
       <c r="M228" s="5" t="s">
         <v>1343</v>
       </c>
       <c r="N228" s="19" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="O228" s="19"/>
       <c r="P228" s="19"/>
@@ -18657,7 +18657,7 @@
         <v>E08b</v>
       </c>
       <c r="K229" s="5" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="L229" s="5" t="s">
         <v>1199</v>
@@ -18666,7 +18666,7 @@
         <v>1342</v>
       </c>
       <c r="N229" s="19" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="O229" s="19"/>
       <c r="P229" s="19"/>
@@ -18690,7 +18690,7 @@
         <v>142</v>
       </c>
       <c r="D230" s="5" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="E230" s="71"/>
       <c r="F230" s="6" t="s">
@@ -18711,16 +18711,16 @@
         <v>E08c</v>
       </c>
       <c r="K230" s="5" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="L230" s="5" t="s">
         <v>1223</v>
       </c>
       <c r="M230" s="5" t="s">
+        <v>1481</v>
+      </c>
+      <c r="N230" s="47" t="s">
         <v>1344</v>
-      </c>
-      <c r="N230" s="47" t="s">
-        <v>1345</v>
       </c>
       <c r="O230" s="47"/>
       <c r="P230" s="47"/>
@@ -18755,7 +18755,7 @@
         <v>1206</v>
       </c>
       <c r="E231" s="16" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="F231" s="52" t="s">
         <v>1135</v>
@@ -18772,7 +18772,7 @@
         <v>E99</v>
       </c>
       <c r="K231" s="46" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="L231" s="46" t="s">
         <v>1253</v>
@@ -18793,7 +18793,7 @@
         <v>1211</v>
       </c>
       <c r="E232" s="16" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="F232" s="52" t="s">
         <v>1227</v>
@@ -19162,22 +19162,22 @@
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="75" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="C2" s="75" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="E2" s="75" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="F2" s="75" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="G2" s="75" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="H2" s="75" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="J2" s="75" t="s">
         <v>950</v>
@@ -19185,97 +19185,97 @@
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="75" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="C3" s="75" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="E3" s="75" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="F3" s="75" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="G3" s="75" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="H3" s="75" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="75" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="C4" s="75" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C6" s="75" t="s">
+        <v>1416</v>
+      </c>
+      <c r="E6" s="75" t="s">
+        <v>1360</v>
+      </c>
+      <c r="G6" s="75" t="s">
         <v>1417</v>
-      </c>
-      <c r="E6" s="75" t="s">
-        <v>1361</v>
-      </c>
-      <c r="G6" s="75" t="s">
-        <v>1418</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C7" s="75" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="D7" s="75">
         <v>116</v>
       </c>
       <c r="E7" s="75" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="G7" s="75" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C8" s="75" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D8" s="75">
         <v>118</v>
       </c>
       <c r="E8" s="75" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="G8" s="75" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C9" s="75" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="D9" s="75">
         <v>119</v>
       </c>
       <c r="E9" s="75" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="G9" s="75" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C10" s="75" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="D10" s="75">
         <v>120</v>
       </c>
       <c r="E10" s="75" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="G10" s="75" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="51" x14ac:dyDescent="0.25">

</xml_diff>